<commit_message>
new Version from 2018 (with Web-GUI)
</commit_message>
<xml_diff>
--- a/doc/ModbusIODefinition.xlsx
+++ b/doc/ModbusIODefinition.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\alain\OneDrive - Höhere Fachschule für Technik Mittelland\Robotino\SPSProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roa2\OneDrive - Höhere Fachschule für Technik Mittelland\Robotino\MPSProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="112" documentId="11_65BFE3B6533DFE15D31A6670A189974FFB6C8A56" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{29E2C95F-3A89-4CEB-837E-3D44EEF580F1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20070" windowHeight="19620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16236" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="MidLevelCmd" sheetId="3" r:id="rId1"/>
+    <sheet name="FlowMidLevel" sheetId="6" r:id="rId2"/>
+    <sheet name="LowLev_IONative" sheetId="1" r:id="rId3"/>
+    <sheet name="HighLevel" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="241">
   <si>
     <t>Base Station</t>
   </si>
@@ -243,13 +247,729 @@
   </si>
   <si>
     <t>MPS Typ</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>Action ID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Payload (Word 1 &amp; 2)</t>
+  </si>
+  <si>
+    <t>8 Bit</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>GetBase</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>ERR</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>BUSY</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>DeliverToSlot</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>Kommunikation</t>
+  </si>
+  <si>
+    <t>Kürzel</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Input / Output</t>
+  </si>
+  <si>
+    <t>Kanal</t>
+  </si>
+  <si>
+    <t>Wert</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Gruppe</t>
+  </si>
+  <si>
+    <t>RS1</t>
+  </si>
+  <si>
+    <t>Ringstation 1</t>
+  </si>
+  <si>
+    <t>192.168.2.23</t>
+  </si>
+  <si>
+    <t>Joel, Nicolas Siffert, Marco</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Ringfarbe 1</t>
+  </si>
+  <si>
+    <t>Ringfarbe 2</t>
+  </si>
+  <si>
+    <t>0 Base</t>
+  </si>
+  <si>
+    <t>1 Base</t>
+  </si>
+  <si>
+    <t>2 Base</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Station in Operation</t>
+  </si>
+  <si>
+    <t>Fehler</t>
+  </si>
+  <si>
+    <t>Base im Output</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>Fehlercode &gt; 150</t>
+  </si>
+  <si>
+    <t>FehlerCode</t>
+  </si>
+  <si>
+    <t>RS2</t>
+  </si>
+  <si>
+    <t>Ringstation 2</t>
+  </si>
+  <si>
+    <t>192.168.2.26</t>
+  </si>
+  <si>
+    <t>Damien, Jonathan, Ivan</t>
+  </si>
+  <si>
+    <t>Fehlercode &gt; 250</t>
+  </si>
+  <si>
+    <t>BaseStation</t>
+  </si>
+  <si>
+    <t>192.168.2.27</t>
+  </si>
+  <si>
+    <t>Nicolas Bigler, Josh, Willy</t>
+  </si>
+  <si>
+    <t>Base Rot</t>
+  </si>
+  <si>
+    <t>Base Schwarz</t>
+  </si>
+  <si>
+    <t>Base Silber</t>
+  </si>
+  <si>
+    <t>Fehlercode &gt; 350</t>
+  </si>
+  <si>
+    <t>CapStation</t>
+  </si>
+  <si>
+    <t>192.168.2.24</t>
+  </si>
+  <si>
+    <t>Michael Hürst, Cedric</t>
+  </si>
+  <si>
+    <t>Cap Einlagern</t>
+  </si>
+  <si>
+    <t>Cap Auslagern</t>
+  </si>
+  <si>
+    <t>Fehlercode &gt; 450</t>
+  </si>
+  <si>
+    <t>DeliveryStation</t>
+  </si>
+  <si>
+    <t>192.168.2.28</t>
+  </si>
+  <si>
+    <t>Benj, Michael Bielmeier, Markus</t>
+  </si>
+  <si>
+    <t>Einlagern in 1</t>
+  </si>
+  <si>
+    <t>Einlagern in 2</t>
+  </si>
+  <si>
+    <t>Einlagern in 3</t>
+  </si>
+  <si>
+    <t>Teil Im Output</t>
+  </si>
+  <si>
+    <t>Fehlercode &gt; 550</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>GetProduct</t>
+  </si>
+  <si>
+    <t>WaitForXBases</t>
+  </si>
+  <si>
+    <t>BandOnUntil</t>
+  </si>
+  <si>
+    <t>1=in//3=out</t>
+  </si>
+  <si>
+    <t>1=in/2=mid/3=out</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>0=off/1=on/2=blink</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>Word 2</t>
+  </si>
+  <si>
+    <t>Word 1</t>
+  </si>
+  <si>
+    <t>Word 0</t>
+  </si>
+  <si>
+    <t>0=always/&gt;0=time in s</t>
+  </si>
+  <si>
+    <t>Festo MPS Commands  over Modbus TCP (from Edison/Refbox)</t>
+  </si>
+  <si>
+    <t>1=BS/2=RS/3=CS/4=DS/5=SS</t>
+  </si>
+  <si>
+    <t>Corresponding RefboxMsg</t>
+  </si>
+  <si>
+    <t>MoveConveyerBelt</t>
+  </si>
+  <si>
+    <t>SetSignalLight</t>
+  </si>
+  <si>
+    <t>BSPushBase</t>
+  </si>
+  <si>
+    <t>SSTask</t>
+  </si>
+  <si>
+    <t>RSMountRing</t>
+  </si>
+  <si>
+    <t>CSTask</t>
+  </si>
+  <si>
+    <t>DSActivateGate</t>
+  </si>
+  <si>
+    <t>NoJob</t>
+  </si>
+  <si>
+    <t>MPS</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>MachineTyp</t>
+  </si>
+  <si>
+    <t>MountRing</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>1=retrieve/2=mount</t>
+  </si>
+  <si>
+    <t>Sobald das Busy-Signal von der MPS wieder auf den Outputregistern(MPS) zurückkommt</t>
+  </si>
+  <si>
+    <t>Output-Lichtschranke steht. (ready). Der Job/Action ist erst beendet, sobald dies abgeholt wurde</t>
+  </si>
+  <si>
+    <t>Robotino</t>
+  </si>
+  <si>
+    <t>RefBox</t>
+  </si>
+  <si>
+    <t>Edison</t>
+  </si>
+  <si>
+    <t>à</t>
+  </si>
+  <si>
+    <t>(Redblink 3s)</t>
+  </si>
+  <si>
+    <r>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21,2,3,Bsy=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+  </si>
+  <si>
+    <t>Start Action</t>
+  </si>
+  <si>
+    <r>
+      <t>ß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21,2,3,Bsy=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21,2,3,Bsy=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+  </si>
+  <si>
+    <t>PrepareMsg</t>
+  </si>
+  <si>
+    <r>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>302,3,0,Bsy=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>302,3,0,Bsy=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>302,3,0,Bsy=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21,2,3,Bsy=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <t>ß</t>
+  </si>
+  <si>
+    <t>Wait 4 Bsy return</t>
+  </si>
+  <si>
+    <t>Wait 4 Busy release</t>
+  </si>
+  <si>
+    <r>
+      <t>ß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…Bsy=1,Rdy=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <t>MPSFinished</t>
+  </si>
+  <si>
+    <r>
+      <t>ß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…Bsy=1,Err=1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <t>Bsp2</t>
+  </si>
+  <si>
+    <t>Bsp1</t>
+  </si>
+  <si>
+    <r>
+      <t>ß</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…Bsy=0,Rdy=0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ß</t>
+    </r>
+  </si>
+  <si>
+    <t>MPSProductRetrieve</t>
+  </si>
+  <si>
+    <t>Wait4BusyRelease
+MPSFinished</t>
+  </si>
+  <si>
+    <t>Wait 4 Rdy/Err/BsyRel</t>
+  </si>
+  <si>
+    <t>MPSFinished 
+(blinkt aber u.U. noch)</t>
+  </si>
+  <si>
+    <t>Prod at Output</t>
+  </si>
+  <si>
+    <t>Prod Retrieved</t>
+  </si>
+  <si>
+    <t>1=dirToOut/2=dirToIn</t>
+  </si>
+  <si>
+    <t>Error Nr</t>
+  </si>
+  <si>
+    <t>Word0</t>
+  </si>
+  <si>
+    <t>Word1</t>
+  </si>
+  <si>
+    <t>Word2</t>
+  </si>
+  <si>
+    <t>Word3</t>
+  </si>
+  <si>
+    <t>Payload</t>
+  </si>
+  <si>
+    <t>Word4</t>
+  </si>
+  <si>
+    <t>Action ID Lights</t>
+  </si>
+  <si>
+    <t>Action ID Machines</t>
+  </si>
+  <si>
+    <t>Word5</t>
+  </si>
+  <si>
+    <t>Word6</t>
+  </si>
+  <si>
+    <t>Word7</t>
+  </si>
+  <si>
+    <t>Word8</t>
+  </si>
+  <si>
+    <t>Word9</t>
+  </si>
+  <si>
+    <t>Slide Counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State </t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>ErrorNr</t>
+  </si>
+  <si>
+    <t>Überlegung für neue Lösung (ev. MidLevel)</t>
+  </si>
+  <si>
+    <t>Word 4</t>
+  </si>
+  <si>
+    <t>Das Ready-Signal wird MPS seitig gesetzt, bei Band-Operationen, sofern das Produkt fertig abholbereit in der</t>
+  </si>
+  <si>
+    <t>Für das Modbus-Protokoll braucht es zwingend ein «Handshake». Und zwar folgendermassen:</t>
+  </si>
+  <si>
+    <t>Graphische Erklärung; siehe 2tes. Register/Reiter "FlowMidLevel"</t>
+  </si>
+  <si>
+    <t>Vollständige Logik in MPSen</t>
+  </si>
+  <si>
+    <t>PRODREADY</t>
+  </si>
+  <si>
+    <t>Beim Senden einer Aktion vom RasPi auf die MPS wird Busy gesetzt.</t>
+  </si>
+  <si>
+    <t>muss es zurückgesetzt werden damit auch eine identische neue Aktion erkannt werden kann.</t>
+  </si>
+  <si>
+    <t>(Lichtschranke frei), und erst jetzt wird Busy MPS-seitig zurückgesetzt.</t>
+  </si>
+  <si>
+    <t>Selbstredend kann auch nur eine Aktion gleichzeitig verarbeitet werden (ist ja dasselbe Band).</t>
+  </si>
+  <si>
+    <t>Ein Queuing müsste falls gewünscht auf dem RasPi-Relay passieren.</t>
+  </si>
+  <si>
+    <t>New ModBus Reg Slide-Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +985,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +1075,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -306,11 +1108,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -327,6 +1190,155 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -640,33 +1652,1314 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:S42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="23" customWidth="1"/>
+    <col min="9" max="15" width="2.21875" style="23" customWidth="1"/>
+    <col min="16" max="16" width="2.109375" customWidth="1"/>
+    <col min="17" max="17" width="8.21875" customWidth="1"/>
+    <col min="18" max="18" width="13.77734375" customWidth="1"/>
+    <col min="20" max="20" width="18.5546875" customWidth="1"/>
+    <col min="21" max="21" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="3.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:19" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="R3" s="57" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="61"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="70"/>
+      <c r="G4" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="70"/>
+      <c r="I4" s="29">
+        <v>7</v>
+      </c>
+      <c r="J4" s="18">
+        <v>6</v>
+      </c>
+      <c r="K4" s="18">
+        <v>5</v>
+      </c>
+      <c r="L4" s="18">
+        <v>4</v>
+      </c>
+      <c r="M4" s="18">
+        <v>3</v>
+      </c>
+      <c r="N4" s="18">
+        <v>2</v>
+      </c>
+      <c r="O4" s="18">
+        <v>1</v>
+      </c>
+      <c r="P4" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="60" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="61"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="35"/>
+    </row>
+    <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61"/>
+      <c r="B6" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0</v>
+      </c>
+      <c r="E6" s="62"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="36"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="61"/>
+      <c r="B7" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="21">
+        <v>10</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" s="63"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="36"/>
+    </row>
+    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="61"/>
+      <c r="B8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="34">
+        <v>20</v>
+      </c>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="36"/>
+    </row>
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="54">
+        <v>21</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="63"/>
+      <c r="G9" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" s="63"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="36"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="34">
+        <v>22</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" s="63"/>
+      <c r="G10" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" s="63"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="59"/>
+      <c r="S10" s="36"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="34">
+        <v>23</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="63"/>
+      <c r="G11" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="H11" s="63"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="37"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="61"/>
+      <c r="B12" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="21">
+        <v>100</v>
+      </c>
+      <c r="E12" s="62"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="36"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="21">
+        <v>101</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="37"/>
+    </row>
+    <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="34">
+        <v>102</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="74"/>
+      <c r="G14" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" s="67"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="59"/>
+      <c r="S14" s="36"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="61"/>
+      <c r="B15" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="21">
+        <v>200</v>
+      </c>
+      <c r="E15" s="62"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="36"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="61"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="21">
+        <v>201</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="37"/>
+    </row>
+    <row r="17" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="21">
+        <v>202</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="74"/>
+      <c r="G17" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" s="67"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="36"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="61" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="21">
+        <v>203</v>
+      </c>
+      <c r="E18" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="36"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="61"/>
+      <c r="B19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="21">
+        <v>300</v>
+      </c>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="36"/>
+    </row>
+    <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="21">
+        <v>302</v>
+      </c>
+      <c r="E20" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="74"/>
+      <c r="G20" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="H20" s="67"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="36"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="34">
+        <v>301</v>
+      </c>
+      <c r="E21" s="73" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="74"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="36"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="61"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="36"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="61"/>
+      <c r="B23" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="21">
+        <v>400</v>
+      </c>
+      <c r="E23" s="62"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="36"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="21">
+        <v>401</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="63"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="36"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="61"/>
+      <c r="B25" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="21">
+        <v>500</v>
+      </c>
+      <c r="E25" s="62"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="36"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="21">
+        <v>501</v>
+      </c>
+      <c r="E26" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="36"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="61"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="36"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="61"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="36"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72" t="s">
+        <v>214</v>
+      </c>
+      <c r="J29" s="72"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="72"/>
+      <c r="R29" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="S29" s="38"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="R30" s="38"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="R31" s="38"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="41" t="s">
+        <v>235</v>
+      </c>
+      <c r="R32" s="38"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="41" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="41" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="41" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="41" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="54">
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:Q29"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I3:P3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+  </mergeCells>
+  <pageMargins left="0.9055118110236221" right="0.70866141732283472" top="0.78740157480314965" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="78" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A3:I24"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="3.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="2.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="53"/>
+      <c r="B3" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="I3" s="53"/>
+    </row>
+    <row r="4" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="I4" s="50"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="50"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="75"/>
+      <c r="I6" s="50"/>
+    </row>
+    <row r="7" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="50"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="H8" s="75" t="s">
+        <v>196</v>
+      </c>
+      <c r="I8" s="50"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="50"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="50"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="H10" s="75"/>
+      <c r="I10" s="50"/>
+    </row>
+    <row r="11" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="50"/>
+    </row>
+    <row r="12" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="50"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="I13" s="50"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="50"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="50"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="50"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="H15" s="76"/>
+      <c r="I15" s="50"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="50"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="50"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="50"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="50"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="50"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="50"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="50"/>
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="H19" t="s">
+        <v>207</v>
+      </c>
+      <c r="I19" s="50"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="50"/>
+      <c r="I20" s="50"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="50"/>
+      <c r="F21" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="50"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="46"/>
+      <c r="I22" s="50"/>
+    </row>
+    <row r="23" spans="1:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="50"/>
+      <c r="D23" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>208</v>
+      </c>
+      <c r="I23" s="50"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="F15:F17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="7" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="7" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
         <v>0</v>
@@ -684,7 +2977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>70</v>
       </c>
@@ -696,8 +2989,8 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="3">
@@ -718,7 +3011,7 @@
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>1</v>
@@ -736,7 +3029,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3">
         <v>2</v>
@@ -754,7 +3047,7 @@
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>3</v>
@@ -768,7 +3061,7 @@
       </c>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3">
         <v>4</v>
@@ -782,7 +3075,7 @@
       </c>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3">
         <v>5</v>
@@ -802,7 +3095,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3">
         <v>6</v>
@@ -822,7 +3115,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3">
         <v>7</v>
@@ -842,7 +3135,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3">
         <v>8</v>
@@ -860,7 +3153,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3">
         <v>9</v>
@@ -878,7 +3171,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3">
         <v>10</v>
@@ -896,7 +3189,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3">
         <v>11</v>
@@ -912,7 +3205,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3">
         <v>12</v>
@@ -928,7 +3221,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3">
         <v>13</v>
@@ -940,7 +3233,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3">
         <v>14</v>
@@ -952,7 +3245,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3">
         <v>15</v>
@@ -964,8 +3257,8 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="2">
@@ -980,7 +3273,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2">
         <v>1</v>
@@ -994,7 +3287,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2">
         <v>2</v>
@@ -1008,7 +3301,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2">
         <v>3</v>
@@ -1022,7 +3315,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2">
         <v>4</v>
@@ -1036,7 +3329,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2">
         <v>5</v>
@@ -1048,7 +3341,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
         <v>6</v>
@@ -1060,7 +3353,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2">
         <v>7</v>
@@ -1072,30 +3365,31 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="14">
         <v>1</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="14">
         <v>2</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="14">
         <v>3</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="14">
         <v>4</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1103,7 +3397,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>68</v>
       </c>
@@ -1114,7 +3408,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -1124,7 +3418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
@@ -1145,7 +3439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4">
         <v>1</v>
@@ -1164,7 +3458,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4">
         <v>2</v>
@@ -1183,7 +3477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4">
         <v>3</v>
@@ -1200,7 +3494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4">
         <v>4</v>
@@ -1219,7 +3513,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4">
         <v>5</v>
@@ -1238,7 +3532,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4">
         <v>6</v>
@@ -1255,7 +3549,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4">
         <v>7</v>
@@ -1272,7 +3566,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4">
         <v>8</v>
@@ -1285,7 +3579,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4">
         <v>9</v>
@@ -1298,7 +3592,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4">
         <v>10</v>
@@ -1315,7 +3609,7 @@
       </c>
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4">
         <v>11</v>
@@ -1330,7 +3624,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4">
         <v>12</v>
@@ -1343,7 +3637,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4">
         <v>13</v>
@@ -1354,7 +3648,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4">
         <v>14</v>
@@ -1365,7 +3659,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4">
         <v>15</v>
@@ -1377,7 +3671,916 @@
       <c r="G48" s="4"/>
     </row>
   </sheetData>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.98425196850393704" bottom="0.98425196850393704" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H72"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="8" style="23" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="30" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D4" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="23">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>101</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="23">
+        <v>1</v>
+      </c>
+      <c r="F6" s="32">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1</v>
+      </c>
+      <c r="F7" s="32">
+        <v>103</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="23">
+        <v>1</v>
+      </c>
+      <c r="F8" s="32">
+        <v>104</v>
+      </c>
+      <c r="G8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D9" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D11" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>111</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D15" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>113</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="23">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="23">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+      <c r="G18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="23">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>201</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="23">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>204</v>
+      </c>
+      <c r="G20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="23">
+        <v>1</v>
+      </c>
+      <c r="F21" s="32">
+        <v>203</v>
+      </c>
+      <c r="G21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="23">
+        <v>1</v>
+      </c>
+      <c r="F22" s="32">
+        <v>204</v>
+      </c>
+      <c r="G22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>205</v>
+      </c>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>210</v>
+      </c>
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="23">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>211</v>
+      </c>
+      <c r="G25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="23">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>212</v>
+      </c>
+      <c r="G26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="23">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>213</v>
+      </c>
+      <c r="G27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D28" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="23">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D30" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="23">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>300</v>
+      </c>
+      <c r="G30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D31" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="23">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>301</v>
+      </c>
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D32" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="23">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>302</v>
+      </c>
+      <c r="G32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D33" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="23">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>305</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D34" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="23">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>310</v>
+      </c>
+      <c r="G34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="23">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>311</v>
+      </c>
+      <c r="G35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D36" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="23">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>312</v>
+      </c>
+      <c r="G36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D37" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="23">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>313</v>
+      </c>
+      <c r="G37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D38" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="23">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" t="s">
+        <v>133</v>
+      </c>
+      <c r="H39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D40" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="23">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>400</v>
+      </c>
+      <c r="G40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D41" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="23">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>401</v>
+      </c>
+      <c r="G41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D42" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="23">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>405</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D43" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="23">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>410</v>
+      </c>
+      <c r="G43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D44" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="23">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>411</v>
+      </c>
+      <c r="G44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D45" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="23">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>412</v>
+      </c>
+      <c r="G45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D46" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" s="23">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>413</v>
+      </c>
+      <c r="G46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D47" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" s="23">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" t="s">
+        <v>139</v>
+      </c>
+      <c r="H48" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D49" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="23">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>500</v>
+      </c>
+      <c r="G49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D50" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E50" s="23">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>501</v>
+      </c>
+      <c r="G50" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D51" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="23">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>502</v>
+      </c>
+      <c r="G51" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D52" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" s="23">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>505</v>
+      </c>
+      <c r="G52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D53" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="23">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>510</v>
+      </c>
+      <c r="G53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D54" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="23">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>511</v>
+      </c>
+      <c r="G54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D55" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E55" s="23">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>512</v>
+      </c>
+      <c r="G55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D56" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" s="23">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>513</v>
+      </c>
+      <c r="G56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D57" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" s="23">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>145</v>
+      </c>
+      <c r="G57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B63" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B64" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B65" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B66" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" s="55" t="s">
+        <v>227</v>
+      </c>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B72" s="56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>